<commit_message>
initial manuscript draft done
</commit_message>
<xml_diff>
--- a/data/areacount.xlsx
+++ b/data/areacount.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="64" uniqueCount="18">
   <si>
     <t>area451</t>
   </si>
@@ -406,954 +406,960 @@
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="true"/>
-    <col min="2" max="3" width="13.85546875" customWidth="true"/>
-    <col min="4" max="5" width="15.28515625" customWidth="true"/>
-    <col min="6" max="7" width="16.85546875" customWidth="true"/>
-    <col min="8" max="9" width="14.5703125" customWidth="true"/>
-    <col min="10" max="11" width="17.42578125" customWidth="true"/>
-    <col min="12" max="13" width="15.140625" customWidth="true"/>
+    <col min="2" max="2" width="13.85546875" customWidth="true"/>
+    <col min="4" max="4" width="15.28515625" customWidth="true"/>
+    <col min="6" max="6" width="16.85546875" customWidth="true"/>
+    <col min="8" max="8" width="14.5703125" customWidth="true"/>
+    <col min="10" max="10" width="17.42578125" customWidth="true"/>
+    <col min="12" max="12" width="15.140625" customWidth="true"/>
+    <col min="3" max="3" width="13.85546875" customWidth="true"/>
+    <col min="5" max="5" width="15.28515625" customWidth="true"/>
+    <col min="7" max="7" width="16.85546875" customWidth="true"/>
+    <col min="9" max="9" width="14.5703125" customWidth="true"/>
+    <col min="11" max="11" width="17.42578125" customWidth="true"/>
+    <col min="13" max="13" width="15.140625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" s="0">
         <v>2002</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>168877750000</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>156519750000</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>0.29628226161003113</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>0.28453746438026428</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>11.341005325317383</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>10.509437561035156</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0">
         <v>11.525702476501465</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>10.99815559387207</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="0">
         <v>4.3607802391052246</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="0">
         <v>5.3234272003173828</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="0">
         <v>3.779853343963623</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="0">
         <v>4.5355572700500488</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3">
+      <c r="A3" s="0">
         <v>2003</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>211598250000</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>198241500000</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>0.28870195150375366</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>0.27817258238792419</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>12.124224662780762</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>10.923653602600098</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0">
         <v>13.018429756164551</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <v>12.294719696044922</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="0">
         <v>6.8356533050537109</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="0">
         <v>8.7052221298217773</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="0">
         <v>6.9046854972839355</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="0">
         <v>8.5402441024780273</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4">
+      <c r="A4" s="0">
         <v>2004</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>193850000000</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>179265500000</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>0.30676984786987305</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>0.29552444815635681</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>10.540505409240723</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>9.659637451171875</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0">
         <v>11.457140922546387</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>10.845796585083008</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="0">
         <v>5.4514007568359375</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="0">
         <v>6.7585005760192871</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="0">
         <v>4.8968782424926758</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="0">
         <v>5.8432421684265137</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5">
+      <c r="A5" s="0">
         <v>2005</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>194553500000</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <v>182500250000</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>0.28377488255500793</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>0.27313092350959778</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>12.300359725952148</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>11.391330718994141</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0">
         <v>12.376280784606934</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>11.754088401794434</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="0">
         <v>4.5137753486633301</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="0">
         <v>5.5040707588195801</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="0">
         <v>3.9735338687896729</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="0">
         <v>4.7725019454956055</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6">
+      <c r="A6" s="0">
         <v>2006</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>175280000000</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <v>163790500000</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>0.29486101865768433</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>0.28433185815811157</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>10.639404296875</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>9.7409696578979492</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0">
         <v>10.867709159851074</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="0">
         <v>10.20331859588623</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="0">
         <v>4.4167590141296387</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="0">
         <v>5.4643597602844238</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="0">
         <v>4.0311870574951172</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="0">
         <v>4.8752322196960449</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7">
+      <c r="A7" s="0">
         <v>2007</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>201615500000</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>189149250000</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="0">
         <v>0.27814149856567383</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>0.26714274287223816</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>15.149476051330566</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>14.024137496948242</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0">
         <v>14.246997833251953</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="0">
         <v>13.624951362609863</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="0">
         <v>4.6140103340148926</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="0">
         <v>5.7799739837646484</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="0">
         <v>4.3024649620056152</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="0">
         <v>5.3205885887145996</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8">
+      <c r="A8" s="0">
         <v>2008</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>209047250000</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <v>196407250000</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="0">
         <v>0.28543657064437866</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>0.27517151832580566</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>14.650535583496094</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>13.345174789428711</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="0">
         <v>13.832075119018555</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="0">
         <v>13.070735931396484</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="0">
         <v>5.5377769470214844</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="0">
         <v>6.9109501838684082</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="0">
         <v>5.1969351768493652</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="0">
         <v>6.2691335678100586</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9">
+      <c r="A9" s="0">
         <v>2009</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>168423250000</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0">
         <v>156185500000</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="0">
         <v>0.30055788159370422</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="0">
         <v>0.28923860192298889</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>15.177305221557617</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>13.882206916809082</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="0">
         <v>14.137123107910156</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="0">
         <v>13.350317001342773</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="0">
         <v>5.4407138824462891</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="0">
         <v>6.7232265472412109</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="0">
         <v>5.0212068557739258</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="0">
         <v>5.967498779296875</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10">
+      <c r="A10" s="0">
         <v>2010</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <v>217596500000</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <v>204300500000</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="0">
         <v>0.27265223860740662</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="0">
         <v>0.26143619418144226</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="0">
         <v>16.650976181030273</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="0">
         <v>15.583359718322754</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="0">
         <v>15.643441200256348</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="0">
         <v>14.957568168640137</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="0">
         <v>5.1833977699279785</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="0">
         <v>6.4765210151672363</v>
       </c>
-      <c r="L10">
-        <v>5.0400466918945313</v>
-      </c>
-      <c r="M10">
+      <c r="L10" s="0">
+        <v>5.0400466918945312</v>
+      </c>
+      <c r="M10" s="0">
         <v>6.1289033889770508</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11">
+      <c r="A11" s="0">
         <v>2011</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0">
         <v>228134000000</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="0">
         <v>214585500000</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="0">
         <v>0.27770078182220459</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="0">
         <v>0.26713964343070984</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="0">
         <v>14.577024459838867</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="0">
         <v>13.255284309387207</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="0">
         <v>13.034558296203613</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="0">
         <v>12.335856437683105</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="0">
         <v>6.247279167175293</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="0">
         <v>7.7013826370239258</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="0">
         <v>5.5048637390136719</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="0">
         <v>6.4365777969360352</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12">
+      <c r="A12" s="0">
         <v>2012</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="0">
         <v>259427500000</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="0">
         <v>243593250000</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="0">
         <v>0.27616226673126221</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="0">
         <v>0.26518663763999939</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="0">
         <v>14.823100090026855</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="0">
         <v>13.685543060302734</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="0">
         <v>13.683866500854492</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="0">
         <v>13.001743316650391</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="0">
         <v>5.0130171775817871</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="0">
         <v>6.1990337371826172</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="0">
         <v>4.4742159843444824</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="0">
         <v>5.3163642883300781</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13">
+      <c r="A13" s="0">
         <v>2013</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="0">
         <v>180876500000</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="0">
         <v>168520750000</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="0">
         <v>0.27979463338851929</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="0">
         <v>0.26768624782562256</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>11.372776031494141</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="0">
         <v>10.452128410339355</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0">
         <v>11.424531936645508</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="0">
         <v>10.852258682250977</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="0">
         <v>5.3982830047607422</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="0">
         <v>6.5484104156494141</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="0">
         <v>4.9671077728271484</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="0">
         <v>5.8484616279602051</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14">
+      <c r="A14" s="0">
         <v>2014</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="0">
         <v>209220000000</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="0">
         <v>195916250000</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="0">
         <v>0.27063620090484619</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="0">
         <v>0.25880074501037598</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0">
         <v>13.521408081054688</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="0">
         <v>12.527207374572754</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="0">
         <v>13.314404487609863</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="0">
         <v>12.729153633117676</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="0">
         <v>4.6849737167358398</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="0">
         <v>5.7673506736755371</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="0">
         <v>4.200681209564209</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="0">
         <v>5.1349244117736816</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15">
+      <c r="A15" s="0">
         <v>2015</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="0">
         <v>184138750000</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="0">
         <v>168951000000</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="0">
         <v>0.29519078135490417</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="0">
         <v>0.28172314167022705</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>11.731015205383301</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="0">
         <v>10.642233848571777</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="0">
         <v>11.835628509521484</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="0">
         <v>11.21085262298584</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="0">
         <v>5.0936279296875</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="0">
         <v>6.2341346740722656</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="0">
         <v>4.5469236373901367</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="0">
         <v>5.5078449249267578</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16">
+      <c r="A16" s="0">
         <v>2016</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="0">
         <v>219364500000</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="0">
         <v>211305000000</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="0">
         <v>0.18593613803386688</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="0">
         <v>0.17604996263980865</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>15.837806701660156</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="0">
         <v>14.480271339416504</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="0">
         <v>15.827577590942383</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="0">
         <v>15.046557426452637</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="0">
         <v>4.0596027374267578</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="0">
         <v>4.8781404495239258</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="0">
         <v>4.0993633270263672</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="0">
         <v>4.9048819541931152</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17">
+      <c r="A17" s="0">
         <v>2017</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="0">
         <v>174047000000</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="0">
         <v>167638500000</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="0">
         <v>0.20896382629871368</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="0">
         <v>0.1999395489692688</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>11.874516487121582</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="0">
         <v>10.706130027770996</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="0">
         <v>11.635966300964355</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="0">
         <v>10.876312255859375</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="0">
         <v>4.1566486358642578</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="0">
         <v>4.9562511444091797</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="0">
         <v>3.901700496673584</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="0">
         <v>4.6539726257324219</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18">
+      <c r="A18" s="0">
         <v>2018</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="0">
         <v>168249500000</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="0">
         <v>159705750000</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="0">
         <v>0.23342999815940857</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="0">
         <v>0.22211289405822754</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>8.6631174087524414</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="0">
         <v>7.86944580078125</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0">
         <v>9.19940185546875</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="0">
         <v>8.6114645004272461</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="0">
         <v>3.6710362434387207</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="0">
         <v>4.3707175254821777</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="0">
         <v>3.3314940929412842</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="0">
         <v>4.003138542175293</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19">
+      <c r="A19" s="0">
         <v>2019</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="0">
         <v>207313750000</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="0">
         <v>198463250000</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="0">
         <v>0.20643576979637146</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="0">
         <v>0.19579559564590454</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>18.524539947509766</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="0">
         <v>16.854597091674805</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0">
         <v>16.50822639465332</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="0">
         <v>15.670439720153809</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="0">
         <v>4.544008731842041</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="0">
         <v>5.5166106224060059</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="0">
         <v>4.504063606262207</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="0">
         <v>5.4487709999084473</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20">
+      <c r="A20" s="0">
         <v>2020</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="0">
         <v>193130000000</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="0">
         <v>183152000000</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="0">
         <v>0.2448686957359314</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="0">
         <v>0.23396597802639008</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>10.648282051086426</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="0">
         <v>9.7670717239379883</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0">
         <v>10.295528411865234</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="0">
         <v>9.774205207824707</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="0">
         <v>4.2171893119812012</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="0">
         <v>5.0317592620849609</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="0">
         <v>3.8565225601196289</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="0">
         <v>4.5219016075134277</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21">
+      <c r="A21" s="0">
         <v>2021</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="0">
         <v>200409250000</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="0">
         <v>188519500000</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="0">
         <v>0.2691347599029541</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="0">
         <v>0.2580416202545166</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="0">
         <v>11.662714004516602</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="0">
         <v>10.87388801574707</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="0">
         <v>11.130527496337891</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="0">
         <v>10.60359001159668</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="0">
         <v>3.8869237899780273</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="0">
         <v>4.720095157623291</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="0">
         <v>3.5384888648986816</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="0">
         <v>4.2752194404602051</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22">
+      <c r="A22" s="0">
         <v>2022</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="0">
         <v>176888750000</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="0">
         <v>165092250000</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="0">
         <v>0.28094872832298279</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="0">
         <v>0.26923063397407532</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="0">
         <v>9.8337688446044922</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="0">
         <v>9.0056781768798828</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="0">
         <v>10.008891105651855</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="0">
         <v>9.5195779800415039</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="0">
         <v>4.2543830871582031</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="0">
         <v>5.1811637878417969</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="0">
         <v>3.7072751522064209</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="0">
         <v>4.4761333465576172</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23">
+      <c r="A23" s="0">
         <v>2023</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="0">
         <v>227432500000</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="0">
         <v>211599500000</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="0">
         <v>0.28568410873413086</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="0">
         <v>0.27376395463943481</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>10.724361419677734</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="0">
         <v>9.9970006942749023</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="0">
         <v>11.521359443664551</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="0">
         <v>11.116439819335938</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="0">
         <v>4.3556880950927734</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="0">
         <v>5.3553552627563477</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="0">
         <v>4.3220434188842773</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="0">
         <v>5.1517801284790039</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor change after review from coauthors
</commit_message>
<xml_diff>
--- a/data/areacount.xlsx
+++ b/data/areacount.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="64" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="189" uniqueCount="24">
   <si>
     <t>area451</t>
   </si>
@@ -80,6 +80,24 @@
   </si>
   <si>
     <t>imcountmasked</t>
+  </si>
+  <si>
+    <t>areaDiff</t>
+  </si>
+  <si>
+    <t>menaDurationDiff</t>
+  </si>
+  <si>
+    <t>stdDurationDiff</t>
+  </si>
+  <si>
+    <t>meanTranstionDiff</t>
+  </si>
+  <si>
+    <t>stdTranstionDiff</t>
+  </si>
+  <si>
+    <t>bareicearea</t>
   </si>
 </sst>
 </file>
@@ -399,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F532BB63-C0C3-48B7-BB7C-D6409CF6D32F}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,17 +425,23 @@
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="true"/>
     <col min="2" max="2" width="13.85546875" customWidth="true"/>
-    <col min="4" max="4" width="15.28515625" customWidth="true"/>
-    <col min="6" max="6" width="16.85546875" customWidth="true"/>
-    <col min="8" max="8" width="14.5703125" customWidth="true"/>
-    <col min="10" max="10" width="17.42578125" customWidth="true"/>
-    <col min="12" max="12" width="15.140625" customWidth="true"/>
+    <col min="4" max="4" width="13.85546875" customWidth="true"/>
+    <col min="6" max="6" width="15.28515625" customWidth="true"/>
+    <col min="8" max="8" width="16.85546875" customWidth="true"/>
+    <col min="10" max="10" width="14.5703125" customWidth="true"/>
+    <col min="12" max="12" width="17.42578125" customWidth="true"/>
     <col min="3" max="3" width="13.85546875" customWidth="true"/>
     <col min="5" max="5" width="15.28515625" customWidth="true"/>
     <col min="7" max="7" width="16.85546875" customWidth="true"/>
     <col min="9" max="9" width="14.5703125" customWidth="true"/>
     <col min="11" max="11" width="17.42578125" customWidth="true"/>
     <col min="13" max="13" width="15.140625" customWidth="true"/>
+    <col min="14" max="14" width="15.140625" customWidth="true"/>
+    <col min="15" max="15" width="15.85546875" customWidth="true"/>
+    <col min="16" max="16" width="17.140625" customWidth="true"/>
+    <col min="17" max="17" width="14.85546875" customWidth="true"/>
+    <col min="18" max="18" width="17.7109375" customWidth="true"/>
+    <col min="19" max="19" width="15.42578125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -425,40 +449,58 @@
         <v>12</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2">
@@ -466,40 +508,58 @@
         <v>2002</v>
       </c>
       <c r="B2" s="0">
+        <v>430319500000</v>
+      </c>
+      <c r="C2" s="0">
         <v>168877750000</v>
       </c>
-      <c r="C2" s="0">
+      <c r="D2" s="0">
         <v>156519750000</v>
       </c>
-      <c r="D2" s="0">
+      <c r="E2" s="0">
         <v>0.29628226161003113</v>
       </c>
-      <c r="E2" s="0">
+      <c r="F2" s="0">
         <v>0.28453746438026428</v>
       </c>
-      <c r="F2" s="0">
+      <c r="G2" s="0">
         <v>11.341005325317383</v>
       </c>
-      <c r="G2" s="0">
+      <c r="H2" s="0">
         <v>10.509437561035156</v>
       </c>
-      <c r="H2" s="0">
+      <c r="I2" s="0">
         <v>11.525702476501465</v>
       </c>
-      <c r="I2" s="0">
+      <c r="J2" s="0">
         <v>10.99815559387207</v>
       </c>
-      <c r="J2" s="0">
+      <c r="K2" s="0">
         <v>4.3607802391052246</v>
       </c>
-      <c r="K2" s="0">
+      <c r="L2" s="0">
         <v>5.3234272003173828</v>
       </c>
-      <c r="L2" s="0">
+      <c r="M2" s="0">
         <v>3.779853343963623</v>
       </c>
-      <c r="M2" s="0">
+      <c r="N2" s="0">
         <v>4.5355572700500488</v>
+      </c>
+      <c r="O2" s="0">
+        <v>12357999616</v>
+      </c>
+      <c r="P2" s="0">
+        <v>1.6281284093856812</v>
+      </c>
+      <c r="Q2" s="0">
+        <v>1.9196090698242188</v>
+      </c>
+      <c r="R2" s="0">
+        <v>-0.96403807401657104</v>
+      </c>
+      <c r="S2" s="0">
+        <v>2.4121148586273193</v>
       </c>
     </row>
     <row r="3">
@@ -507,40 +567,58 @@
         <v>2003</v>
       </c>
       <c r="B3" s="0">
+        <v>464612500000</v>
+      </c>
+      <c r="C3" s="0">
         <v>211598250000</v>
       </c>
-      <c r="C3" s="0">
+      <c r="D3" s="0">
         <v>198241500000</v>
       </c>
-      <c r="D3" s="0">
+      <c r="E3" s="0">
         <v>0.28870195150375366</v>
       </c>
-      <c r="E3" s="0">
+      <c r="F3" s="0">
         <v>0.27817258238792419</v>
       </c>
-      <c r="F3" s="0">
+      <c r="G3" s="0">
         <v>12.124224662780762</v>
       </c>
-      <c r="G3" s="0">
+      <c r="H3" s="0">
         <v>10.923653602600098</v>
       </c>
-      <c r="H3" s="0">
+      <c r="I3" s="0">
         <v>13.018429756164551</v>
       </c>
-      <c r="I3" s="0">
+      <c r="J3" s="0">
         <v>12.294719696044922</v>
       </c>
-      <c r="J3" s="0">
+      <c r="K3" s="0">
         <v>6.8356533050537109</v>
       </c>
-      <c r="K3" s="0">
+      <c r="L3" s="0">
         <v>8.7052221298217773</v>
       </c>
-      <c r="L3" s="0">
+      <c r="M3" s="0">
         <v>6.9046854972839355</v>
       </c>
-      <c r="M3" s="0">
+      <c r="N3" s="0">
         <v>8.5402441024780273</v>
+      </c>
+      <c r="O3" s="0">
+        <v>13356749824</v>
+      </c>
+      <c r="P3" s="0">
+        <v>1.9361371994018555</v>
+      </c>
+      <c r="Q3" s="0">
+        <v>2.4587900638580322</v>
+      </c>
+      <c r="R3" s="0">
+        <v>-1.7786475419998169</v>
+      </c>
+      <c r="S3" s="0">
+        <v>4.5241832733154297</v>
       </c>
     </row>
     <row r="4">
@@ -548,40 +626,58 @@
         <v>2004</v>
       </c>
       <c r="B4" s="0">
+        <v>454987250000</v>
+      </c>
+      <c r="C4" s="0">
         <v>193850000000</v>
       </c>
-      <c r="C4" s="0">
+      <c r="D4" s="0">
         <v>179265500000</v>
       </c>
-      <c r="D4" s="0">
+      <c r="E4" s="0">
         <v>0.30676984786987305</v>
       </c>
-      <c r="E4" s="0">
+      <c r="F4" s="0">
         <v>0.29552444815635681</v>
       </c>
-      <c r="F4" s="0">
+      <c r="G4" s="0">
         <v>10.540505409240723</v>
       </c>
-      <c r="G4" s="0">
+      <c r="H4" s="0">
         <v>9.659637451171875</v>
       </c>
-      <c r="H4" s="0">
+      <c r="I4" s="0">
         <v>11.457140922546387</v>
       </c>
-      <c r="I4" s="0">
+      <c r="J4" s="0">
         <v>10.845796585083008</v>
       </c>
-      <c r="J4" s="0">
+      <c r="K4" s="0">
         <v>5.4514007568359375</v>
       </c>
-      <c r="K4" s="0">
+      <c r="L4" s="0">
         <v>6.7585005760192871</v>
       </c>
-      <c r="L4" s="0">
+      <c r="M4" s="0">
         <v>4.8968782424926758</v>
       </c>
-      <c r="M4" s="0">
+      <c r="N4" s="0">
         <v>5.8432421684265137</v>
+      </c>
+      <c r="O4" s="0">
+        <v>14584500224</v>
+      </c>
+      <c r="P4" s="0">
+        <v>1.6398484706878662</v>
+      </c>
+      <c r="Q4" s="0">
+        <v>1.9840105772018433</v>
+      </c>
+      <c r="R4" s="0">
+        <v>-1.2234562635421753</v>
+      </c>
+      <c r="S4" s="0">
+        <v>2.9568374156951904</v>
       </c>
     </row>
     <row r="5">
@@ -589,40 +685,58 @@
         <v>2005</v>
       </c>
       <c r="B5" s="0">
+        <v>460345250000</v>
+      </c>
+      <c r="C5" s="0">
         <v>194553500000</v>
       </c>
-      <c r="C5" s="0">
+      <c r="D5" s="0">
         <v>182500250000</v>
       </c>
-      <c r="D5" s="0">
+      <c r="E5" s="0">
         <v>0.28377488255500793</v>
       </c>
-      <c r="E5" s="0">
+      <c r="F5" s="0">
         <v>0.27313092350959778</v>
       </c>
-      <c r="F5" s="0">
+      <c r="G5" s="0">
         <v>12.300359725952148</v>
       </c>
-      <c r="G5" s="0">
+      <c r="H5" s="0">
         <v>11.391330718994141</v>
       </c>
-      <c r="H5" s="0">
+      <c r="I5" s="0">
         <v>12.376280784606934</v>
       </c>
-      <c r="I5" s="0">
+      <c r="J5" s="0">
         <v>11.754088401794434</v>
       </c>
-      <c r="J5" s="0">
+      <c r="K5" s="0">
         <v>4.5137753486633301</v>
       </c>
-      <c r="K5" s="0">
+      <c r="L5" s="0">
         <v>5.5040707588195801</v>
       </c>
-      <c r="L5" s="0">
+      <c r="M5" s="0">
         <v>3.9735338687896729</v>
       </c>
-      <c r="M5" s="0">
+      <c r="N5" s="0">
         <v>4.7725019454956055</v>
+      </c>
+      <c r="O5" s="0">
+        <v>12053250048</v>
+      </c>
+      <c r="P5" s="0">
+        <v>1.6414018869400024</v>
+      </c>
+      <c r="Q5" s="0">
+        <v>1.9964249134063721</v>
+      </c>
+      <c r="R5" s="0">
+        <v>-0.94845074415206909</v>
+      </c>
+      <c r="S5" s="0">
+        <v>2.403308629989624</v>
       </c>
     </row>
     <row r="6">
@@ -630,40 +744,58 @@
         <v>2006</v>
       </c>
       <c r="B6" s="0">
+        <v>434377500000</v>
+      </c>
+      <c r="C6" s="0">
         <v>175280000000</v>
       </c>
-      <c r="C6" s="0">
+      <c r="D6" s="0">
         <v>163790500000</v>
       </c>
-      <c r="D6" s="0">
+      <c r="E6" s="0">
         <v>0.29486101865768433</v>
       </c>
-      <c r="E6" s="0">
+      <c r="F6" s="0">
         <v>0.28433185815811157</v>
       </c>
-      <c r="F6" s="0">
+      <c r="G6" s="0">
         <v>10.639404296875</v>
       </c>
-      <c r="G6" s="0">
+      <c r="H6" s="0">
         <v>9.7409696578979492</v>
       </c>
-      <c r="H6" s="0">
+      <c r="I6" s="0">
         <v>10.867709159851074</v>
       </c>
-      <c r="I6" s="0">
+      <c r="J6" s="0">
         <v>10.20331859588623</v>
       </c>
-      <c r="J6" s="0">
+      <c r="K6" s="0">
         <v>4.4167590141296387</v>
       </c>
-      <c r="K6" s="0">
+      <c r="L6" s="0">
         <v>5.4643597602844238</v>
       </c>
-      <c r="L6" s="0">
+      <c r="M6" s="0">
         <v>4.0311870574951172</v>
       </c>
-      <c r="M6" s="0">
+      <c r="N6" s="0">
         <v>4.8752322196960449</v>
+      </c>
+      <c r="O6" s="0">
+        <v>11489500160</v>
+      </c>
+      <c r="P6" s="0">
+        <v>1.5610994100570679</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>1.8878332376480103</v>
+      </c>
+      <c r="R6" s="0">
+        <v>-1.0008807182312012</v>
+      </c>
+      <c r="S6" s="0">
+        <v>2.5149405002593994</v>
       </c>
     </row>
     <row r="7">
@@ -671,40 +803,58 @@
         <v>2007</v>
       </c>
       <c r="B7" s="0">
+        <v>458574000000</v>
+      </c>
+      <c r="C7" s="0">
         <v>201615500000</v>
       </c>
-      <c r="C7" s="0">
+      <c r="D7" s="0">
         <v>189149250000</v>
       </c>
-      <c r="D7" s="0">
+      <c r="E7" s="0">
         <v>0.27814149856567383</v>
       </c>
-      <c r="E7" s="0">
+      <c r="F7" s="0">
         <v>0.26714274287223816</v>
       </c>
-      <c r="F7" s="0">
+      <c r="G7" s="0">
         <v>15.149476051330566</v>
       </c>
-      <c r="G7" s="0">
+      <c r="H7" s="0">
         <v>14.024137496948242</v>
       </c>
-      <c r="H7" s="0">
+      <c r="I7" s="0">
         <v>14.246997833251953</v>
       </c>
-      <c r="I7" s="0">
+      <c r="J7" s="0">
         <v>13.624951362609863</v>
       </c>
-      <c r="J7" s="0">
+      <c r="K7" s="0">
         <v>4.6140103340148926</v>
       </c>
-      <c r="K7" s="0">
+      <c r="L7" s="0">
         <v>5.7799739837646484</v>
       </c>
-      <c r="L7" s="0">
+      <c r="M7" s="0">
         <v>4.3024649620056152</v>
       </c>
-      <c r="M7" s="0">
+      <c r="N7" s="0">
         <v>5.3205885887145996</v>
+      </c>
+      <c r="O7" s="0">
+        <v>12466249728</v>
+      </c>
+      <c r="P7" s="0">
+        <v>2.0415623188018799</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>2.4142124652862549</v>
+      </c>
+      <c r="R7" s="0">
+        <v>-1.1990082263946533</v>
+      </c>
+      <c r="S7" s="0">
+        <v>3.0416915416717529</v>
       </c>
     </row>
     <row r="8">
@@ -712,40 +862,58 @@
         <v>2008</v>
       </c>
       <c r="B8" s="0">
+        <v>467153250000</v>
+      </c>
+      <c r="C8" s="0">
         <v>209047250000</v>
       </c>
-      <c r="C8" s="0">
+      <c r="D8" s="0">
         <v>196407250000</v>
       </c>
-      <c r="D8" s="0">
+      <c r="E8" s="0">
         <v>0.28543657064437866</v>
       </c>
-      <c r="E8" s="0">
+      <c r="F8" s="0">
         <v>0.27517151832580566</v>
       </c>
-      <c r="F8" s="0">
+      <c r="G8" s="0">
         <v>14.650535583496094</v>
       </c>
-      <c r="G8" s="0">
+      <c r="H8" s="0">
         <v>13.345174789428711</v>
       </c>
-      <c r="H8" s="0">
+      <c r="I8" s="0">
         <v>13.832075119018555</v>
       </c>
-      <c r="I8" s="0">
+      <c r="J8" s="0">
         <v>13.070735931396484</v>
       </c>
-      <c r="J8" s="0">
+      <c r="K8" s="0">
         <v>5.5377769470214844</v>
       </c>
-      <c r="K8" s="0">
+      <c r="L8" s="0">
         <v>6.9109501838684082</v>
       </c>
-      <c r="L8" s="0">
+      <c r="M8" s="0">
         <v>5.1969351768493652</v>
       </c>
-      <c r="M8" s="0">
+      <c r="N8" s="0">
         <v>6.2691335678100586</v>
+      </c>
+      <c r="O8" s="0">
+        <v>12640000000</v>
+      </c>
+      <c r="P8" s="0">
+        <v>2.1620955467224121</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>2.4856767654418945</v>
+      </c>
+      <c r="R8" s="0">
+        <v>-1.4025386571884155</v>
+      </c>
+      <c r="S8" s="0">
+        <v>3.3983068466186523</v>
       </c>
     </row>
     <row r="9">
@@ -753,40 +921,58 @@
         <v>2009</v>
       </c>
       <c r="B9" s="0">
+        <v>389162750000</v>
+      </c>
+      <c r="C9" s="0">
         <v>168423250000</v>
       </c>
-      <c r="C9" s="0">
+      <c r="D9" s="0">
         <v>156185500000</v>
       </c>
-      <c r="D9" s="0">
+      <c r="E9" s="0">
         <v>0.30055788159370422</v>
       </c>
-      <c r="E9" s="0">
+      <c r="F9" s="0">
         <v>0.28923860192298889</v>
       </c>
-      <c r="F9" s="0">
+      <c r="G9" s="0">
         <v>15.177305221557617</v>
       </c>
-      <c r="G9" s="0">
+      <c r="H9" s="0">
         <v>13.882206916809082</v>
       </c>
-      <c r="H9" s="0">
+      <c r="I9" s="0">
         <v>14.137123107910156</v>
       </c>
-      <c r="I9" s="0">
+      <c r="J9" s="0">
         <v>13.350317001342773</v>
       </c>
-      <c r="J9" s="0">
+      <c r="K9" s="0">
         <v>5.4407138824462891</v>
       </c>
-      <c r="K9" s="0">
+      <c r="L9" s="0">
         <v>6.7232265472412109</v>
       </c>
-      <c r="L9" s="0">
+      <c r="M9" s="0">
         <v>5.0212068557739258</v>
       </c>
-      <c r="M9" s="0">
+      <c r="N9" s="0">
         <v>5.967498779296875</v>
+      </c>
+      <c r="O9" s="0">
+        <v>12237750272</v>
+      </c>
+      <c r="P9" s="0">
+        <v>2.3786666393280029</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>2.697246789932251</v>
+      </c>
+      <c r="R9" s="0">
+        <v>-1.3407118320465088</v>
+      </c>
+      <c r="S9" s="0">
+        <v>3.3593063354492188</v>
       </c>
     </row>
     <row r="10">
@@ -794,40 +980,58 @@
         <v>2010</v>
       </c>
       <c r="B10" s="0">
+        <v>485715250000</v>
+      </c>
+      <c r="C10" s="0">
         <v>217596500000</v>
       </c>
-      <c r="C10" s="0">
+      <c r="D10" s="0">
         <v>204300500000</v>
       </c>
-      <c r="D10" s="0">
+      <c r="E10" s="0">
         <v>0.27265223860740662</v>
       </c>
-      <c r="E10" s="0">
+      <c r="F10" s="0">
         <v>0.26143619418144226</v>
       </c>
-      <c r="F10" s="0">
+      <c r="G10" s="0">
         <v>16.650976181030273</v>
       </c>
-      <c r="G10" s="0">
+      <c r="H10" s="0">
         <v>15.583359718322754</v>
       </c>
-      <c r="H10" s="0">
+      <c r="I10" s="0">
         <v>15.643441200256348</v>
       </c>
-      <c r="I10" s="0">
+      <c r="J10" s="0">
         <v>14.957568168640137</v>
       </c>
-      <c r="J10" s="0">
+      <c r="K10" s="0">
         <v>5.1833977699279785</v>
       </c>
-      <c r="K10" s="0">
+      <c r="L10" s="0">
         <v>6.4765210151672363</v>
       </c>
-      <c r="L10" s="0">
+      <c r="M10" s="0">
         <v>5.0400466918945312</v>
       </c>
-      <c r="M10" s="0">
+      <c r="N10" s="0">
         <v>6.1289033889770508</v>
+      </c>
+      <c r="O10" s="0">
+        <v>13296000000</v>
+      </c>
+      <c r="P10" s="0">
+        <v>2.0717864036560059</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>2.5186223983764648</v>
+      </c>
+      <c r="R10" s="0">
+        <v>-1.2992062568664551</v>
+      </c>
+      <c r="S10" s="0">
+        <v>3.2588768005371094</v>
       </c>
     </row>
     <row r="11">
@@ -835,40 +1039,58 @@
         <v>2011</v>
       </c>
       <c r="B11" s="0">
+        <v>463611750000</v>
+      </c>
+      <c r="C11" s="0">
         <v>228134000000</v>
       </c>
-      <c r="C11" s="0">
+      <c r="D11" s="0">
         <v>214585500000</v>
       </c>
-      <c r="D11" s="0">
+      <c r="E11" s="0">
         <v>0.27770078182220459</v>
       </c>
-      <c r="E11" s="0">
+      <c r="F11" s="0">
         <v>0.26713964343070984</v>
       </c>
-      <c r="F11" s="0">
+      <c r="G11" s="0">
         <v>14.577024459838867</v>
       </c>
-      <c r="G11" s="0">
+      <c r="H11" s="0">
         <v>13.255284309387207</v>
       </c>
-      <c r="H11" s="0">
+      <c r="I11" s="0">
         <v>13.034558296203613</v>
       </c>
-      <c r="I11" s="0">
+      <c r="J11" s="0">
         <v>12.335856437683105</v>
       </c>
-      <c r="J11" s="0">
+      <c r="K11" s="0">
         <v>6.247279167175293</v>
       </c>
-      <c r="K11" s="0">
+      <c r="L11" s="0">
         <v>7.7013826370239258</v>
       </c>
-      <c r="L11" s="0">
+      <c r="M11" s="0">
         <v>5.5048637390136719</v>
       </c>
-      <c r="M11" s="0">
+      <c r="N11" s="0">
         <v>6.4365777969360352</v>
+      </c>
+      <c r="O11" s="0">
+        <v>13548499968</v>
+      </c>
+      <c r="P11" s="0">
+        <v>2.1602299213409424</v>
+      </c>
+      <c r="Q11" s="0">
+        <v>2.3429610729217529</v>
+      </c>
+      <c r="R11" s="0">
+        <v>-1.4413695335388184</v>
+      </c>
+      <c r="S11" s="0">
+        <v>3.3071784973144531</v>
       </c>
     </row>
     <row r="12">
@@ -876,40 +1098,58 @@
         <v>2012</v>
       </c>
       <c r="B12" s="0">
+        <v>536036750000</v>
+      </c>
+      <c r="C12" s="0">
         <v>259427500000</v>
       </c>
-      <c r="C12" s="0">
+      <c r="D12" s="0">
         <v>243593250000</v>
       </c>
-      <c r="D12" s="0">
+      <c r="E12" s="0">
         <v>0.27616226673126221</v>
       </c>
-      <c r="E12" s="0">
+      <c r="F12" s="0">
         <v>0.26518663763999939</v>
       </c>
-      <c r="F12" s="0">
+      <c r="G12" s="0">
         <v>14.823100090026855</v>
       </c>
-      <c r="G12" s="0">
+      <c r="H12" s="0">
         <v>13.685543060302734</v>
       </c>
-      <c r="H12" s="0">
+      <c r="I12" s="0">
         <v>13.683866500854492</v>
       </c>
-      <c r="I12" s="0">
+      <c r="J12" s="0">
         <v>13.001743316650391</v>
       </c>
-      <c r="J12" s="0">
+      <c r="K12" s="0">
         <v>5.0130171775817871</v>
       </c>
-      <c r="K12" s="0">
+      <c r="L12" s="0">
         <v>6.1990337371826172</v>
       </c>
-      <c r="L12" s="0">
+      <c r="M12" s="0">
         <v>4.4742159843444824</v>
       </c>
-      <c r="M12" s="0">
+      <c r="N12" s="0">
         <v>5.3163642883300781</v>
+      </c>
+      <c r="O12" s="0">
+        <v>15834250240</v>
+      </c>
+      <c r="P12" s="0">
+        <v>2.0201585292816162</v>
+      </c>
+      <c r="Q12" s="0">
+        <v>2.3485963344573975</v>
+      </c>
+      <c r="R12" s="0">
+        <v>-1.178799033164978</v>
+      </c>
+      <c r="S12" s="0">
+        <v>2.8012151718139648</v>
       </c>
     </row>
     <row r="13">
@@ -917,40 +1157,58 @@
         <v>2013</v>
       </c>
       <c r="B13" s="0">
+        <v>412400500000</v>
+      </c>
+      <c r="C13" s="0">
         <v>180876500000</v>
       </c>
-      <c r="C13" s="0">
+      <c r="D13" s="0">
         <v>168520750000</v>
       </c>
-      <c r="D13" s="0">
+      <c r="E13" s="0">
         <v>0.27979463338851929</v>
       </c>
-      <c r="E13" s="0">
+      <c r="F13" s="0">
         <v>0.26768624782562256</v>
       </c>
-      <c r="F13" s="0">
+      <c r="G13" s="0">
         <v>11.372776031494141</v>
       </c>
-      <c r="G13" s="0">
+      <c r="H13" s="0">
         <v>10.452128410339355</v>
       </c>
-      <c r="H13" s="0">
+      <c r="I13" s="0">
         <v>11.424531936645508</v>
       </c>
-      <c r="I13" s="0">
+      <c r="J13" s="0">
         <v>10.852258682250977</v>
       </c>
-      <c r="J13" s="0">
+      <c r="K13" s="0">
         <v>5.3982830047607422</v>
       </c>
-      <c r="K13" s="0">
+      <c r="L13" s="0">
         <v>6.5484104156494141</v>
       </c>
-      <c r="L13" s="0">
+      <c r="M13" s="0">
         <v>4.9671077728271484</v>
       </c>
-      <c r="M13" s="0">
+      <c r="N13" s="0">
         <v>5.8484616279602051</v>
+      </c>
+      <c r="O13" s="0">
+        <v>12355749888</v>
+      </c>
+      <c r="P13" s="0">
+        <v>1.6612108945846558</v>
+      </c>
+      <c r="Q13" s="0">
+        <v>2.0329217910766602</v>
+      </c>
+      <c r="R13" s="0">
+        <v>-1.1598660945892334</v>
+      </c>
+      <c r="S13" s="0">
+        <v>2.8661301136016846</v>
       </c>
     </row>
     <row r="14">
@@ -958,40 +1216,58 @@
         <v>2014</v>
       </c>
       <c r="B14" s="0">
+        <v>475262500000</v>
+      </c>
+      <c r="C14" s="0">
         <v>209220000000</v>
       </c>
-      <c r="C14" s="0">
+      <c r="D14" s="0">
         <v>195916250000</v>
       </c>
-      <c r="D14" s="0">
+      <c r="E14" s="0">
         <v>0.27063620090484619</v>
       </c>
-      <c r="E14" s="0">
+      <c r="F14" s="0">
         <v>0.25880074501037598</v>
       </c>
-      <c r="F14" s="0">
+      <c r="G14" s="0">
         <v>13.521408081054688</v>
       </c>
-      <c r="G14" s="0">
+      <c r="H14" s="0">
         <v>12.527207374572754</v>
       </c>
-      <c r="H14" s="0">
+      <c r="I14" s="0">
         <v>13.314404487609863</v>
       </c>
-      <c r="I14" s="0">
+      <c r="J14" s="0">
         <v>12.729153633117676</v>
       </c>
-      <c r="J14" s="0">
+      <c r="K14" s="0">
         <v>4.6849737167358398</v>
       </c>
-      <c r="K14" s="0">
+      <c r="L14" s="0">
         <v>5.7673506736755371</v>
       </c>
-      <c r="L14" s="0">
+      <c r="M14" s="0">
         <v>4.200681209564209</v>
       </c>
-      <c r="M14" s="0">
+      <c r="N14" s="0">
         <v>5.1349244117736816</v>
+      </c>
+      <c r="O14" s="0">
+        <v>13303749632</v>
+      </c>
+      <c r="P14" s="0">
+        <v>1.828352689743042</v>
+      </c>
+      <c r="Q14" s="0">
+        <v>2.1800618171691895</v>
+      </c>
+      <c r="R14" s="0">
+        <v>-1.0965464115142822</v>
+      </c>
+      <c r="S14" s="0">
+        <v>2.701791524887085</v>
       </c>
     </row>
     <row r="15">
@@ -999,40 +1275,58 @@
         <v>2015</v>
       </c>
       <c r="B15" s="0">
+        <v>438530250000</v>
+      </c>
+      <c r="C15" s="0">
         <v>184138750000</v>
       </c>
-      <c r="C15" s="0">
+      <c r="D15" s="0">
         <v>168951000000</v>
       </c>
-      <c r="D15" s="0">
+      <c r="E15" s="0">
         <v>0.29519078135490417</v>
       </c>
-      <c r="E15" s="0">
+      <c r="F15" s="0">
         <v>0.28172314167022705</v>
       </c>
-      <c r="F15" s="0">
+      <c r="G15" s="0">
         <v>11.731015205383301</v>
       </c>
-      <c r="G15" s="0">
+      <c r="H15" s="0">
         <v>10.642233848571777</v>
       </c>
-      <c r="H15" s="0">
+      <c r="I15" s="0">
         <v>11.835628509521484</v>
       </c>
-      <c r="I15" s="0">
+      <c r="J15" s="0">
         <v>11.21085262298584</v>
       </c>
-      <c r="J15" s="0">
+      <c r="K15" s="0">
         <v>5.0936279296875</v>
       </c>
-      <c r="K15" s="0">
+      <c r="L15" s="0">
         <v>6.2341346740722656</v>
       </c>
-      <c r="L15" s="0">
+      <c r="M15" s="0">
         <v>4.5469236373901367</v>
       </c>
-      <c r="M15" s="0">
+      <c r="N15" s="0">
         <v>5.5078449249267578</v>
+      </c>
+      <c r="O15" s="0">
+        <v>15187749888</v>
+      </c>
+      <c r="P15" s="0">
+        <v>2.0168406963348389</v>
+      </c>
+      <c r="Q15" s="0">
+        <v>2.2991552352905273</v>
+      </c>
+      <c r="R15" s="0">
+        <v>-1.247808575630188</v>
+      </c>
+      <c r="S15" s="0">
+        <v>3.0154690742492676</v>
       </c>
     </row>
     <row r="16">
@@ -1040,40 +1334,58 @@
         <v>2016</v>
       </c>
       <c r="B16" s="0">
+        <v>503896500000</v>
+      </c>
+      <c r="C16" s="0">
         <v>219364500000</v>
       </c>
-      <c r="C16" s="0">
+      <c r="D16" s="0">
         <v>211305000000</v>
       </c>
-      <c r="D16" s="0">
+      <c r="E16" s="0">
         <v>0.18593613803386688</v>
       </c>
-      <c r="E16" s="0">
+      <c r="F16" s="0">
         <v>0.17604996263980865</v>
       </c>
-      <c r="F16" s="0">
+      <c r="G16" s="0">
         <v>15.837806701660156</v>
       </c>
-      <c r="G16" s="0">
+      <c r="H16" s="0">
         <v>14.480271339416504</v>
       </c>
-      <c r="H16" s="0">
+      <c r="I16" s="0">
         <v>15.827577590942383</v>
       </c>
-      <c r="I16" s="0">
+      <c r="J16" s="0">
         <v>15.046557426452637</v>
       </c>
-      <c r="J16" s="0">
+      <c r="K16" s="0">
         <v>4.0596027374267578</v>
       </c>
-      <c r="K16" s="0">
+      <c r="L16" s="0">
         <v>4.8781404495239258</v>
       </c>
-      <c r="L16" s="0">
+      <c r="M16" s="0">
         <v>4.0993633270263672</v>
       </c>
-      <c r="M16" s="0">
+      <c r="N16" s="0">
         <v>4.9048819541931152</v>
+      </c>
+      <c r="O16" s="0">
+        <v>8059500032</v>
+      </c>
+      <c r="P16" s="0">
+        <v>1.9166382551193237</v>
+      </c>
+      <c r="Q16" s="0">
+        <v>2.5279550552368164</v>
+      </c>
+      <c r="R16" s="0">
+        <v>-0.82888126373291016</v>
+      </c>
+      <c r="S16" s="0">
+        <v>2.4705839157104492</v>
       </c>
     </row>
     <row r="17">
@@ -1081,40 +1393,58 @@
         <v>2017</v>
       </c>
       <c r="B17" s="0">
+        <v>442938750000</v>
+      </c>
+      <c r="C17" s="0">
         <v>174047000000</v>
       </c>
-      <c r="C17" s="0">
+      <c r="D17" s="0">
         <v>167638500000</v>
       </c>
-      <c r="D17" s="0">
+      <c r="E17" s="0">
         <v>0.20896382629871368</v>
       </c>
-      <c r="E17" s="0">
+      <c r="F17" s="0">
         <v>0.1999395489692688</v>
       </c>
-      <c r="F17" s="0">
+      <c r="G17" s="0">
         <v>11.874516487121582</v>
       </c>
-      <c r="G17" s="0">
+      <c r="H17" s="0">
         <v>10.706130027770996</v>
       </c>
-      <c r="H17" s="0">
+      <c r="I17" s="0">
         <v>11.635966300964355</v>
       </c>
-      <c r="I17" s="0">
+      <c r="J17" s="0">
         <v>10.876312255859375</v>
       </c>
-      <c r="J17" s="0">
+      <c r="K17" s="0">
         <v>4.1566486358642578</v>
       </c>
-      <c r="K17" s="0">
+      <c r="L17" s="0">
         <v>4.9562511444091797</v>
       </c>
-      <c r="L17" s="0">
+      <c r="M17" s="0">
         <v>3.901700496673584</v>
       </c>
-      <c r="M17" s="0">
+      <c r="N17" s="0">
         <v>4.6539726257324219</v>
+      </c>
+      <c r="O17" s="0">
+        <v>6408500224</v>
+      </c>
+      <c r="P17" s="0">
+        <v>1.5762056112289429</v>
+      </c>
+      <c r="Q17" s="0">
+        <v>1.9512373208999634</v>
+      </c>
+      <c r="R17" s="0">
+        <v>-0.80137914419174194</v>
+      </c>
+      <c r="S17" s="0">
+        <v>2.2316832542419434</v>
       </c>
     </row>
     <row r="18">
@@ -1122,40 +1452,58 @@
         <v>2018</v>
       </c>
       <c r="B18" s="0">
+        <v>429972750000</v>
+      </c>
+      <c r="C18" s="0">
         <v>168249500000</v>
       </c>
-      <c r="C18" s="0">
+      <c r="D18" s="0">
         <v>159705750000</v>
       </c>
-      <c r="D18" s="0">
+      <c r="E18" s="0">
         <v>0.23342999815940857</v>
       </c>
-      <c r="E18" s="0">
+      <c r="F18" s="0">
         <v>0.22211289405822754</v>
       </c>
-      <c r="F18" s="0">
+      <c r="G18" s="0">
         <v>8.6631174087524414</v>
       </c>
-      <c r="G18" s="0">
+      <c r="H18" s="0">
         <v>7.86944580078125</v>
       </c>
-      <c r="H18" s="0">
+      <c r="I18" s="0">
         <v>9.19940185546875</v>
       </c>
-      <c r="I18" s="0">
+      <c r="J18" s="0">
         <v>8.6114645004272461</v>
       </c>
-      <c r="J18" s="0">
+      <c r="K18" s="0">
         <v>3.6710362434387207</v>
       </c>
-      <c r="K18" s="0">
+      <c r="L18" s="0">
         <v>4.3707175254821777</v>
       </c>
-      <c r="L18" s="0">
+      <c r="M18" s="0">
         <v>3.3314940929412842</v>
       </c>
-      <c r="M18" s="0">
+      <c r="N18" s="0">
         <v>4.003138542175293</v>
+      </c>
+      <c r="O18" s="0">
+        <v>8543750144</v>
+      </c>
+      <c r="P18" s="0">
+        <v>1.1935590505599976</v>
+      </c>
+      <c r="Q18" s="0">
+        <v>1.5820915699005127</v>
+      </c>
+      <c r="R18" s="0">
+        <v>-0.68055629730224609</v>
+      </c>
+      <c r="S18" s="0">
+        <v>1.9243093729019165</v>
       </c>
     </row>
     <row r="19">
@@ -1163,40 +1511,58 @@
         <v>2019</v>
       </c>
       <c r="B19" s="0">
+        <v>482984750000</v>
+      </c>
+      <c r="C19" s="0">
         <v>207313750000</v>
       </c>
-      <c r="C19" s="0">
+      <c r="D19" s="0">
         <v>198463250000</v>
       </c>
-      <c r="D19" s="0">
+      <c r="E19" s="0">
         <v>0.20643576979637146</v>
       </c>
-      <c r="E19" s="0">
+      <c r="F19" s="0">
         <v>0.19579559564590454</v>
       </c>
-      <c r="F19" s="0">
+      <c r="G19" s="0">
         <v>18.524539947509766</v>
       </c>
-      <c r="G19" s="0">
+      <c r="H19" s="0">
         <v>16.854597091674805</v>
       </c>
-      <c r="H19" s="0">
+      <c r="I19" s="0">
         <v>16.50822639465332</v>
       </c>
-      <c r="I19" s="0">
+      <c r="J19" s="0">
         <v>15.670439720153809</v>
       </c>
-      <c r="J19" s="0">
+      <c r="K19" s="0">
         <v>4.544008731842041</v>
       </c>
-      <c r="K19" s="0">
+      <c r="L19" s="0">
         <v>5.5166106224060059</v>
       </c>
-      <c r="L19" s="0">
+      <c r="M19" s="0">
         <v>4.504063606262207</v>
       </c>
-      <c r="M19" s="0">
+      <c r="N19" s="0">
         <v>5.4487709999084473</v>
+      </c>
+      <c r="O19" s="0">
+        <v>8850499584</v>
+      </c>
+      <c r="P19" s="0">
+        <v>2.4398925304412842</v>
+      </c>
+      <c r="Q19" s="0">
+        <v>2.867927074432373</v>
+      </c>
+      <c r="R19" s="0">
+        <v>-1.0447589159011841</v>
+      </c>
+      <c r="S19" s="0">
+        <v>2.8588802814483643</v>
       </c>
     </row>
     <row r="20">
@@ -1204,40 +1570,58 @@
         <v>2020</v>
       </c>
       <c r="B20" s="0">
+        <v>445193000000</v>
+      </c>
+      <c r="C20" s="0">
         <v>193130000000</v>
       </c>
-      <c r="C20" s="0">
+      <c r="D20" s="0">
         <v>183152000000</v>
       </c>
-      <c r="D20" s="0">
+      <c r="E20" s="0">
         <v>0.2448686957359314</v>
       </c>
-      <c r="E20" s="0">
+      <c r="F20" s="0">
         <v>0.23396597802639008</v>
       </c>
-      <c r="F20" s="0">
+      <c r="G20" s="0">
         <v>10.648282051086426</v>
       </c>
-      <c r="G20" s="0">
+      <c r="H20" s="0">
         <v>9.7670717239379883</v>
       </c>
-      <c r="H20" s="0">
+      <c r="I20" s="0">
         <v>10.295528411865234</v>
       </c>
-      <c r="I20" s="0">
+      <c r="J20" s="0">
         <v>9.774205207824707</v>
       </c>
-      <c r="J20" s="0">
+      <c r="K20" s="0">
         <v>4.2171893119812012</v>
       </c>
-      <c r="K20" s="0">
+      <c r="L20" s="0">
         <v>5.0317592620849609</v>
       </c>
-      <c r="L20" s="0">
+      <c r="M20" s="0">
         <v>3.8565225601196289</v>
       </c>
-      <c r="M20" s="0">
+      <c r="N20" s="0">
         <v>4.5219016075134277</v>
+      </c>
+      <c r="O20" s="0">
+        <v>9978000384</v>
+      </c>
+      <c r="P20" s="0">
+        <v>1.3950966596603394</v>
+      </c>
+      <c r="Q20" s="0">
+        <v>1.7943320274353027</v>
+      </c>
+      <c r="R20" s="0">
+        <v>-0.82018625736236572</v>
+      </c>
+      <c r="S20" s="0">
+        <v>2.1559238433837891</v>
       </c>
     </row>
     <row r="21">
@@ -1245,40 +1629,58 @@
         <v>2021</v>
       </c>
       <c r="B21" s="0">
+        <v>468141250000</v>
+      </c>
+      <c r="C21" s="0">
         <v>200409250000</v>
       </c>
-      <c r="C21" s="0">
+      <c r="D21" s="0">
         <v>188519500000</v>
       </c>
-      <c r="D21" s="0">
+      <c r="E21" s="0">
         <v>0.2691347599029541</v>
       </c>
-      <c r="E21" s="0">
+      <c r="F21" s="0">
         <v>0.2580416202545166</v>
       </c>
-      <c r="F21" s="0">
+      <c r="G21" s="0">
         <v>11.662714004516602</v>
       </c>
-      <c r="G21" s="0">
+      <c r="H21" s="0">
         <v>10.87388801574707</v>
       </c>
-      <c r="H21" s="0">
+      <c r="I21" s="0">
         <v>11.130527496337891</v>
       </c>
-      <c r="I21" s="0">
+      <c r="J21" s="0">
         <v>10.60359001159668</v>
       </c>
-      <c r="J21" s="0">
+      <c r="K21" s="0">
         <v>3.8869237899780273</v>
       </c>
-      <c r="K21" s="0">
+      <c r="L21" s="0">
         <v>4.720095157623291</v>
       </c>
-      <c r="L21" s="0">
+      <c r="M21" s="0">
         <v>3.5384888648986816</v>
       </c>
-      <c r="M21" s="0">
+      <c r="N21" s="0">
         <v>4.2752194404602051</v>
+      </c>
+      <c r="O21" s="0">
+        <v>11889750016</v>
+      </c>
+      <c r="P21" s="0">
+        <v>1.4477123022079468</v>
+      </c>
+      <c r="Q21" s="0">
+        <v>1.796625018119812</v>
+      </c>
+      <c r="R21" s="0">
+        <v>-0.80263048410415649</v>
+      </c>
+      <c r="S21" s="0">
+        <v>2.1259720325469971</v>
       </c>
     </row>
     <row r="22">
@@ -1286,40 +1688,58 @@
         <v>2022</v>
       </c>
       <c r="B22" s="0">
+        <v>423621250000</v>
+      </c>
+      <c r="C22" s="0">
         <v>176888750000</v>
       </c>
-      <c r="C22" s="0">
+      <c r="D22" s="0">
         <v>165092250000</v>
       </c>
-      <c r="D22" s="0">
+      <c r="E22" s="0">
         <v>0.28094872832298279</v>
       </c>
-      <c r="E22" s="0">
+      <c r="F22" s="0">
         <v>0.26923063397407532</v>
       </c>
-      <c r="F22" s="0">
+      <c r="G22" s="0">
         <v>9.8337688446044922</v>
       </c>
-      <c r="G22" s="0">
+      <c r="H22" s="0">
         <v>9.0056781768798828</v>
       </c>
-      <c r="H22" s="0">
+      <c r="I22" s="0">
         <v>10.008891105651855</v>
       </c>
-      <c r="I22" s="0">
+      <c r="J22" s="0">
         <v>9.5195779800415039</v>
       </c>
-      <c r="J22" s="0">
+      <c r="K22" s="0">
         <v>4.2543830871582031</v>
       </c>
-      <c r="K22" s="0">
+      <c r="L22" s="0">
         <v>5.1811637878417969</v>
       </c>
-      <c r="L22" s="0">
+      <c r="M22" s="0">
         <v>3.7072751522064209</v>
       </c>
-      <c r="M22" s="0">
+      <c r="N22" s="0">
         <v>4.4761333465576172</v>
+      </c>
+      <c r="O22" s="0">
+        <v>11796500480</v>
+      </c>
+      <c r="P22" s="0">
+        <v>1.4417756795883179</v>
+      </c>
+      <c r="Q22" s="0">
+        <v>1.7242289781570435</v>
+      </c>
+      <c r="R22" s="0">
+        <v>-0.92910325527191162</v>
+      </c>
+      <c r="S22" s="0">
+        <v>2.2970349788665771</v>
       </c>
     </row>
     <row r="23">
@@ -1327,40 +1747,58 @@
         <v>2023</v>
       </c>
       <c r="B23" s="0">
+        <v>512583250000</v>
+      </c>
+      <c r="C23" s="0">
         <v>227432500000</v>
       </c>
-      <c r="C23" s="0">
+      <c r="D23" s="0">
         <v>211599500000</v>
       </c>
-      <c r="D23" s="0">
+      <c r="E23" s="0">
         <v>0.28568410873413086</v>
       </c>
-      <c r="E23" s="0">
+      <c r="F23" s="0">
         <v>0.27376395463943481</v>
       </c>
-      <c r="F23" s="0">
+      <c r="G23" s="0">
         <v>10.724361419677734</v>
       </c>
-      <c r="G23" s="0">
+      <c r="H23" s="0">
         <v>9.9970006942749023</v>
       </c>
-      <c r="H23" s="0">
+      <c r="I23" s="0">
         <v>11.521359443664551</v>
       </c>
-      <c r="I23" s="0">
+      <c r="J23" s="0">
         <v>11.116439819335938</v>
       </c>
-      <c r="J23" s="0">
+      <c r="K23" s="0">
         <v>4.3556880950927734</v>
       </c>
-      <c r="K23" s="0">
+      <c r="L23" s="0">
         <v>5.3553552627563477</v>
       </c>
-      <c r="L23" s="0">
+      <c r="M23" s="0">
         <v>4.3220434188842773</v>
       </c>
-      <c r="M23" s="0">
+      <c r="N23" s="0">
         <v>5.1517801284790039</v>
+      </c>
+      <c r="O23" s="0">
+        <v>15832999936</v>
+      </c>
+      <c r="P23" s="0">
+        <v>1.4390959739685059</v>
+      </c>
+      <c r="Q23" s="0">
+        <v>1.8297257423400879</v>
+      </c>
+      <c r="R23" s="0">
+        <v>-1.0057739019393921</v>
+      </c>
+      <c r="S23" s="0">
+        <v>2.7764639854431152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>